<commit_message>
Corrige errores visuales y restaura encabezado en AdminPanel
</commit_message>
<xml_diff>
--- a/Inventario_SevenShoes1.xlsx
+++ b/Inventario_SevenShoes1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t>Nombre</t>
   </si>
@@ -113,13 +113,22 @@
   </si>
   <si>
     <t>85464548794524365875461320323000002450</t>
+  </si>
+  <si>
+    <t>05/02/2025</t>
+  </si>
+  <si>
+    <t>500004050</t>
+  </si>
+  <si>
+    <t>VIZ M 520 TACO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +143,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -185,6 +201,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,6 +750,29 @@
         <v>17</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2">
+        <v>555458585</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="5">
+        <v>20639</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="260" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización total: WebSocket, ruta /emitir, frontend sincronizado con Android
</commit_message>
<xml_diff>
--- a/Inventario_SevenShoes1.xlsx
+++ b/Inventario_SevenShoes1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>Nombre</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>VIZ M 520 TACO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prueba </t>
+  </si>
+  <si>
+    <t>05/02/2026</t>
+  </si>
+  <si>
+    <t>nike</t>
+  </si>
+  <si>
+    <t>45919158</t>
   </si>
 </sst>
 </file>
@@ -503,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,6 +785,26 @@
         <v>17</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4242</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="2">
+        <v>54524224</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="260" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>

<commit_message>
✅ Correcciones en Reportes.jsx: uso correcto de user.correo y user.empresa
</commit_message>
<xml_diff>
--- a/Inventario_SevenShoes1.xlsx
+++ b/Inventario_SevenShoes1.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>Código Barras</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -34,9 +31,6 @@
     <t>RFID</t>
   </si>
   <si>
-    <t>Ubicación</t>
-  </si>
-  <si>
     <t>500004041</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
     <t>8885554642152461945421240000000000000</t>
   </si>
   <si>
-    <t>85464548794524365875461320323000002450</t>
-  </si>
-  <si>
     <t>05/02/2025</t>
   </si>
   <si>
@@ -134,6 +125,24 @@
   </si>
   <si>
     <t>45919158</t>
+  </si>
+  <si>
+    <t>Prueba 2</t>
+  </si>
+  <si>
+    <t>Puma</t>
+  </si>
+  <si>
+    <t>8546450004524365875461320323000002450</t>
+  </si>
+  <si>
+    <t>8546454879452365875461320323000002450</t>
+  </si>
+  <si>
+    <t>Ubicacion</t>
+  </si>
+  <si>
+    <t>Codigo</t>
   </si>
 </sst>
 </file>
@@ -515,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,272 +546,298 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
         <v>555888999</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="2">
         <v>555888998</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
         <v>555888997</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
         <v>555888996</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
         <v>555888995</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2">
         <v>555888994</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2">
         <v>555888993</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
         <v>555888992</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2">
         <v>555888991</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2">
         <v>555458585</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" s="5">
         <v>20639</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2">
         <v>4242</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2">
         <v>54524224</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45454545</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2">
+        <v>15245863</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>